<commit_message>
Cambio de tipo de gráfico en el excel
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p2/P2_UO277876.xlsx
+++ b/src/main/java/algestudiante/p2/P2_UO277876.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC8CC46-C5BB-414B-BCB7-60019BB63436}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC247CC-0BCA-4214-BE2E-39DCBB1D108F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
@@ -12053,15 +12053,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13534,8 +13534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5628303C-3F20-4835-AC65-1A4FE3A04F85}">
   <dimension ref="A2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Cambios en los tiempos del mediana a tres y incorporación del pdf
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p2/P2_UO277876.xlsx
+++ b/src/main/java/algestudiante/p2/P2_UO277876.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC247CC-0BCA-4214-BE2E-39DCBB1D108F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FBC00A-DB32-4507-B554-FB69B0DBCDAE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Insercción" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
   <si>
     <t>nVeces</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t xml:space="preserve">nVeces = 1000 </t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -309,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -358,6 +361,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1391,61 +1403,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>2.92E-2</c:v>
+                  <c:v>1.54E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8000000000000001E-2</c:v>
+                  <c:v>2.87E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.8699999999999996E-2</c:v>
+                  <c:v>5.3900000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26100000000000001</c:v>
+                  <c:v>0.10050000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.72089999999999999</c:v>
+                  <c:v>0.21529999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5982000000000001</c:v>
+                  <c:v>0.45390000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2774000000000001</c:v>
+                  <c:v>0.97330000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.8852000000000002</c:v>
+                  <c:v>2.0991</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.056800000000001</c:v>
+                  <c:v>4.5570000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.707000000000001</c:v>
+                  <c:v>8.8857999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62.27</c:v>
+                  <c:v>18.637699999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>129.56800000000001</c:v>
+                  <c:v>39.780999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>290.93</c:v>
+                  <c:v>83.77</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>631.33000000000004</c:v>
+                  <c:v>172.33500000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1245.82</c:v>
+                  <c:v>364.93</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3140.2</c:v>
+                  <c:v>764.02</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6335</c:v>
+                  <c:v>1572.89</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13311</c:v>
+                  <c:v>3549.4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>56223</c:v>
+                  <c:v>7409</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1830,61 +1842,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>1.8800000000000001E-2</c:v>
+                  <c:v>2.47E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2800000000000003E-2</c:v>
+                  <c:v>4.0300000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.3100000000000001E-2</c:v>
+                  <c:v>7.1599999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1016</c:v>
+                  <c:v>0.16439999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.2172</c:v>
+                  <c:v>0.56230000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.4708</c:v>
+                  <c:v>1.2765</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0104</c:v>
+                  <c:v>2.6608000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1743999999999999</c:v>
+                  <c:v>6.0510999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.6412000000000004</c:v>
+                  <c:v>12.6121</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.885300000000001</c:v>
+                  <c:v>33.930999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>31.89</c:v>
+                  <c:v>97.686000000000007</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>80.915999999999997</c:v>
+                  <c:v>190.12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>218.803</c:v>
+                  <c:v>500.03</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>755.31</c:v>
+                  <c:v>1488.58</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2525.86</c:v>
+                  <c:v>6867.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5722.1</c:v>
+                  <c:v>24163.7</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9638</c:v>
+                  <c:v>29810</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24260</c:v>
+                  <c:v>80771</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>66922</c:v>
+                  <c:v>248324</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12428,8 +12440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50AC779-C55D-4822-8A6D-58AA05F2A758}">
   <dimension ref="A2:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B21"/>
+    <sheetView topLeftCell="E13" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12859,8 +12871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B473716-F3A2-49BD-996D-A970964813E6}">
   <dimension ref="A2:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12874,7 +12886,7 @@
       <c r="A2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="12" t="s">
@@ -12904,7 +12916,7 @@
       <c r="A3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="32">
         <v>1000</v>
       </c>
       <c r="C3" s="29">
@@ -12935,7 +12947,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="18"/>
-      <c r="B4" s="29">
+      <c r="B4" s="32">
         <v>2000</v>
       </c>
       <c r="C4" s="29">
@@ -12962,7 +12974,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="18"/>
-      <c r="B5" s="29">
+      <c r="B5" s="32">
         <v>4000</v>
       </c>
       <c r="C5" s="29">
@@ -12985,7 +12997,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
-      <c r="B6" s="29">
+      <c r="B6" s="32">
         <v>8000</v>
       </c>
       <c r="C6" s="29">
@@ -13008,7 +13020,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
-      <c r="B7" s="29">
+      <c r="B7" s="32">
         <v>16000</v>
       </c>
       <c r="C7" s="29">
@@ -13033,7 +13045,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="18"/>
-      <c r="B8" s="29">
+      <c r="B8" s="32">
         <v>32000</v>
       </c>
       <c r="C8" s="29">
@@ -13060,7 +13072,7 @@
       <c r="A9" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="29">
+      <c r="B9" s="32">
         <v>64000</v>
       </c>
       <c r="C9" s="29">
@@ -13087,7 +13099,7 @@
       <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="32">
         <v>128000</v>
       </c>
       <c r="C10" s="29">
@@ -13105,6 +13117,9 @@
       <c r="F10" s="18"/>
       <c r="G10" s="16" t="s">
         <v>17</v>
+      </c>
+      <c r="K10" t="s">
+        <v>22</v>
       </c>
       <c r="N10" s="21">
         <v>1</v>
@@ -13114,7 +13129,7 @@
       <c r="A11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="29">
+      <c r="B11" s="32">
         <v>256000</v>
       </c>
       <c r="C11" s="29">
@@ -13138,7 +13153,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
-      <c r="B12" s="29">
+      <c r="B12" s="32">
         <v>512000</v>
       </c>
       <c r="C12" s="29">
@@ -13155,7 +13170,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
-      <c r="B13" s="30">
+      <c r="B13" s="33">
         <v>1024000</v>
       </c>
       <c r="C13" s="30">
@@ -13185,10 +13200,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2212FF28-3494-42A9-B9A1-1E9767DE072A}">
-  <dimension ref="A2:N18"/>
+  <dimension ref="A2:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13509,7 +13524,7 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -13517,11 +13532,16 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
       <c r="E18" s="31"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="L30" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13534,8 +13554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5628303C-3F20-4835-AC65-1A4FE3A04F85}">
   <dimension ref="A2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13587,12 +13607,12 @@
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="D3" s="29">
-        <f>292/N6</f>
-        <v>2.92E-2</v>
+        <f>154/N6</f>
+        <v>1.54E-2</v>
       </c>
       <c r="E3" s="29">
-        <f>188/N6</f>
-        <v>1.8800000000000001E-2</v>
+        <f>247/N6</f>
+        <v>2.47E-2</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>12</v>
@@ -13618,12 +13638,12 @@
         <v>3.9199999999999999E-2</v>
       </c>
       <c r="D4" s="29">
-        <f>480/N6</f>
-        <v>4.8000000000000001E-2</v>
+        <f>287/N6</f>
+        <v>2.87E-2</v>
       </c>
       <c r="E4" s="29">
-        <f>328/N6</f>
-        <v>3.2800000000000003E-2</v>
+        <f>403/N6</f>
+        <v>4.0300000000000002E-2</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="16"/>
@@ -13645,12 +13665,12 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="D5" s="29">
-        <f>987/N6</f>
-        <v>9.8699999999999996E-2</v>
+        <f>539/N6</f>
+        <v>5.3900000000000003E-2</v>
       </c>
       <c r="E5" s="29">
-        <f>531/N6</f>
-        <v>5.3100000000000001E-2</v>
+        <f>716/N6</f>
+        <v>7.1599999999999997E-2</v>
       </c>
       <c r="F5" s="18"/>
       <c r="G5" s="16"/>
@@ -13668,12 +13688,12 @@
         <v>0.1104</v>
       </c>
       <c r="D6" s="29">
-        <f>2610/N6</f>
-        <v>0.26100000000000001</v>
+        <f>1005/N6</f>
+        <v>0.10050000000000001</v>
       </c>
       <c r="E6" s="29">
-        <f>1016/N6</f>
-        <v>0.1016</v>
+        <f>1644/N6</f>
+        <v>0.16439999999999999</v>
       </c>
       <c r="F6" s="18"/>
       <c r="G6" s="16"/>
@@ -13691,12 +13711,12 @@
         <v>0.37880000000000003</v>
       </c>
       <c r="D7" s="29">
-        <f>7209/N6</f>
-        <v>0.72089999999999999</v>
+        <f>2153/N6</f>
+        <v>0.21529999999999999</v>
       </c>
       <c r="E7" s="29">
-        <f>2172/N6</f>
-        <v>0.2172</v>
+        <f>5623/N6</f>
+        <v>0.56230000000000002</v>
       </c>
       <c r="F7" s="18"/>
       <c r="G7" s="16"/>
@@ -13714,12 +13734,12 @@
         <v>1.0757000000000001</v>
       </c>
       <c r="D8" s="29">
-        <f>15982/N6</f>
-        <v>1.5982000000000001</v>
+        <f>4539/N6</f>
+        <v>0.45390000000000003</v>
       </c>
       <c r="E8" s="29">
-        <f>4708/N6</f>
-        <v>0.4708</v>
+        <f>12765/N6</f>
+        <v>1.2765</v>
       </c>
       <c r="F8" s="18"/>
       <c r="G8" s="16"/>
@@ -13737,12 +13757,12 @@
         <v>2.2686000000000002</v>
       </c>
       <c r="D9" s="29">
-        <f>32774/N6</f>
-        <v>3.2774000000000001</v>
+        <f>9733/N6</f>
+        <v>0.97330000000000005</v>
       </c>
       <c r="E9" s="29">
-        <f>10104/N6</f>
-        <v>1.0104</v>
+        <f>26608/N6</f>
+        <v>2.6608000000000001</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="16"/>
@@ -13760,12 +13780,12 @@
         <v>5.0964</v>
       </c>
       <c r="D10" s="29">
-        <f>68852/N6</f>
-        <v>6.8852000000000002</v>
+        <f>20991/N6</f>
+        <v>2.0991</v>
       </c>
       <c r="E10" s="29">
-        <f>21744/N6</f>
-        <v>2.1743999999999999</v>
+        <f>60511/N6</f>
+        <v>6.0510999999999999</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="16"/>
@@ -13783,12 +13803,12 @@
         <v>10.363</v>
       </c>
       <c r="D11" s="29">
-        <f>140568/N6</f>
-        <v>14.056800000000001</v>
+        <f>45570/N6</f>
+        <v>4.5570000000000004</v>
       </c>
       <c r="E11" s="29">
-        <f>46412/N6</f>
-        <v>4.6412000000000004</v>
+        <f>126121/N6</f>
+        <v>12.6121</v>
       </c>
       <c r="F11" s="18"/>
       <c r="G11" s="16"/>
@@ -13805,17 +13825,17 @@
         <v>26.72</v>
       </c>
       <c r="D12" s="29">
-        <f>29707/N7</f>
-        <v>29.707000000000001</v>
+        <f>88858/N6</f>
+        <v>8.8857999999999997</v>
       </c>
       <c r="E12" s="29">
-        <f>108853/N6</f>
-        <v>10.885300000000001</v>
-      </c>
-      <c r="F12" s="18" t="s">
+        <f>33931/N7</f>
+        <v>33.930999999999997</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
@@ -13827,17 +13847,15 @@
         <v>60.363</v>
       </c>
       <c r="D13" s="29">
-        <f>62270/N7</f>
-        <v>62.27</v>
+        <f>186377/N6</f>
+        <v>18.637699999999999</v>
       </c>
       <c r="E13" s="29">
-        <f>31890/N7</f>
-        <v>31.89</v>
+        <f>97686/N7</f>
+        <v>97.686000000000007</v>
       </c>
       <c r="F13" s="18"/>
-      <c r="G13" s="16" t="s">
-        <v>21</v>
-      </c>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
@@ -13849,14 +13867,16 @@
         <v>116.51</v>
       </c>
       <c r="D14" s="29">
-        <f>129568/N7</f>
-        <v>129.56800000000001</v>
+        <f>39781/N7</f>
+        <v>39.780999999999999</v>
       </c>
       <c r="E14" s="29">
-        <f>80916/N7</f>
-        <v>80.915999999999997</v>
-      </c>
-      <c r="F14" s="18"/>
+        <f>190120/N7</f>
+        <v>190.12</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>13</v>
+      </c>
       <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -13871,17 +13891,17 @@
         <v>275.81</v>
       </c>
       <c r="D15" s="29">
-        <f>29093/N8</f>
-        <v>290.93</v>
+        <f>83770/N7</f>
+        <v>83.77</v>
       </c>
       <c r="E15" s="29">
-        <f>218803/N7</f>
-        <v>218.803</v>
-      </c>
-      <c r="F15" s="18" t="s">
+        <f>50003/N8</f>
+        <v>500.03</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
@@ -13893,17 +13913,15 @@
         <v>564.30999999999995</v>
       </c>
       <c r="D16" s="29">
-        <f>63133/N8</f>
-        <v>631.33000000000004</v>
+        <f>172335/N7</f>
+        <v>172.33500000000001</v>
       </c>
       <c r="E16" s="29">
-        <f>75531/N8</f>
-        <v>755.31</v>
+        <f>148858/N8</f>
+        <v>1488.58</v>
       </c>
       <c r="F16" s="18"/>
-      <c r="G16" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
@@ -13915,15 +13933,19 @@
         <v>1144.1600000000001</v>
       </c>
       <c r="D17" s="29">
-        <f>124582/N8</f>
-        <v>1245.82</v>
+        <f>36493/N8</f>
+        <v>364.93</v>
       </c>
       <c r="E17" s="29">
-        <f>252586/N8</f>
-        <v>2525.86</v>
-      </c>
-      <c r="F17" s="18"/>
-      <c r="G17" s="16"/>
+        <f>68673/N9</f>
+        <v>6867.3</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
@@ -13937,19 +13959,15 @@
         <v>2422.1999999999998</v>
       </c>
       <c r="D18" s="29">
-        <f>31402/N9</f>
-        <v>3140.2</v>
+        <f>76402/N8</f>
+        <v>764.02</v>
       </c>
       <c r="E18" s="29">
-        <f>57221/N9</f>
-        <v>5722.1</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>17</v>
-      </c>
+        <f>241637/N9</f>
+        <v>24163.7</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
@@ -13961,11 +13979,12 @@
         <v>4875.2</v>
       </c>
       <c r="D19" s="29">
-        <f>63350/N9</f>
-        <v>6335</v>
+        <f>157289/N8</f>
+        <v>1572.89</v>
       </c>
       <c r="E19" s="29">
-        <v>9638</v>
+        <f>29810/N10</f>
+        <v>29810</v>
       </c>
       <c r="F19" s="18"/>
       <c r="G19" s="16" t="s">
@@ -13982,14 +14001,16 @@
         <v>9949.1</v>
       </c>
       <c r="D20" s="29">
-        <f>133110/N9</f>
-        <v>13311</v>
+        <f>35494/N9</f>
+        <v>3549.4</v>
       </c>
       <c r="E20" s="29">
-        <f>24260/N10</f>
-        <v>24260</v>
-      </c>
-      <c r="F20" s="3"/>
+        <f>80771/N10</f>
+        <v>80771</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>17</v>
+      </c>
       <c r="G20" s="16"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -14002,16 +14023,14 @@
         <v>20405.2</v>
       </c>
       <c r="D21" s="30">
-        <f>56223/N10</f>
-        <v>56223</v>
-      </c>
-      <c r="E21" s="30">
-        <f>66922/N10</f>
-        <v>66922</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>18</v>
-      </c>
+        <f>74090/N9</f>
+        <v>7409</v>
+      </c>
+      <c r="E21" s="34">
+        <f>248324/N10</f>
+        <v>248324</v>
+      </c>
+      <c r="F21" s="19"/>
       <c r="G21" s="27"/>
     </row>
   </sheetData>

</xml_diff>